<commit_message>
Update gantt-chart_L version 2.xlsx
</commit_message>
<xml_diff>
--- a/gantt-chart_L version 2.xlsx
+++ b/gantt-chart_L version 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HTCS5607\HTCS 5607 IS Application Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HTCS5607\HTCS5607\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BA74191-CD64-41DA-A262-7F2B7677CA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD96CD1-4333-4E5B-BD5E-54AB44CDB2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4074,7 +4074,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F68" sqref="F68"/>
+      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5039,7 +5039,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="62">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I10" s="63">
         <f t="shared" si="4"/>
@@ -5126,7 +5126,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="63">
         <f t="shared" si="4"/>
@@ -5211,7 +5211,9 @@
       <c r="G12" s="61">
         <v>1</v>
       </c>
-      <c r="H12" s="62"/>
+      <c r="H12" s="62">
+        <v>1</v>
+      </c>
       <c r="I12" s="63">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5295,7 +5297,9 @@
       <c r="G13" s="61">
         <v>1</v>
       </c>
-      <c r="H13" s="62"/>
+      <c r="H13" s="62">
+        <v>1</v>
+      </c>
       <c r="I13" s="63">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5379,7 +5383,9 @@
       <c r="G14" s="61">
         <v>1</v>
       </c>
-      <c r="H14" s="62"/>
+      <c r="H14" s="62">
+        <v>1</v>
+      </c>
       <c r="I14" s="63">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5463,7 +5469,9 @@
       <c r="G15" s="61">
         <v>1</v>
       </c>
-      <c r="H15" s="62"/>
+      <c r="H15" s="62">
+        <v>1</v>
+      </c>
       <c r="I15" s="63">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5547,7 +5555,9 @@
       <c r="G16" s="61">
         <v>1</v>
       </c>
-      <c r="H16" s="62"/>
+      <c r="H16" s="62">
+        <v>1</v>
+      </c>
       <c r="I16" s="63">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5631,7 +5641,9 @@
       <c r="G17" s="61">
         <v>1</v>
       </c>
-      <c r="H17" s="62"/>
+      <c r="H17" s="62">
+        <v>1</v>
+      </c>
       <c r="I17" s="63">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -5715,7 +5727,9 @@
       <c r="G18" s="61">
         <v>1</v>
       </c>
-      <c r="H18" s="62"/>
+      <c r="H18" s="62">
+        <v>1</v>
+      </c>
       <c r="I18" s="63">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5799,7 +5813,9 @@
       <c r="G19" s="61">
         <v>1</v>
       </c>
-      <c r="H19" s="62"/>
+      <c r="H19" s="62">
+        <v>1</v>
+      </c>
       <c r="I19" s="63">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -5885,7 +5901,7 @@
         <v>2</v>
       </c>
       <c r="H20" s="62">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I20" s="63">
         <f t="shared" si="4"/>
@@ -5970,7 +5986,9 @@
       <c r="G21" s="61">
         <v>1</v>
       </c>
-      <c r="H21" s="62"/>
+      <c r="H21" s="62">
+        <v>1</v>
+      </c>
       <c r="I21" s="63">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -6056,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="63">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
finished with class diagram and activity diagrams
</commit_message>
<xml_diff>
--- a/gantt-chart_L version 2.xlsx
+++ b/gantt-chart_L version 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HTCS5607\HTCS5607\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22522D7-0422-4A40-8C77-F7456DC76B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBD35E7-77F3-4CD2-B594-8ABC18232E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3198,13 +3198,6 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3214,10 +3207,6 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="166" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3226,6 +3215,17 @@
     </xf>
     <xf numFmtId="166" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4073,8 +4073,8 @@
   <dimension ref="A1:BN101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4102,29 +4102,29 @@
       <c r="E1" s="152"/>
       <c r="F1" s="152"/>
       <c r="I1" s="121"/>
-      <c r="K1" s="177" t="s">
+      <c r="K1" s="183" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="177"/>
-      <c r="M1" s="177"/>
-      <c r="N1" s="177"/>
-      <c r="O1" s="177"/>
-      <c r="P1" s="177"/>
-      <c r="Q1" s="177"/>
-      <c r="R1" s="177"/>
-      <c r="S1" s="177"/>
-      <c r="T1" s="177"/>
-      <c r="U1" s="177"/>
-      <c r="V1" s="177"/>
-      <c r="W1" s="177"/>
-      <c r="X1" s="177"/>
-      <c r="Y1" s="177"/>
-      <c r="Z1" s="177"/>
-      <c r="AA1" s="177"/>
-      <c r="AB1" s="177"/>
-      <c r="AC1" s="177"/>
-      <c r="AD1" s="177"/>
-      <c r="AE1" s="177"/>
+      <c r="L1" s="183"/>
+      <c r="M1" s="183"/>
+      <c r="N1" s="183"/>
+      <c r="O1" s="183"/>
+      <c r="P1" s="183"/>
+      <c r="Q1" s="183"/>
+      <c r="R1" s="183"/>
+      <c r="S1" s="183"/>
+      <c r="T1" s="183"/>
+      <c r="U1" s="183"/>
+      <c r="V1" s="183"/>
+      <c r="W1" s="183"/>
+      <c r="X1" s="183"/>
+      <c r="Y1" s="183"/>
+      <c r="Z1" s="183"/>
+      <c r="AA1" s="183"/>
+      <c r="AB1" s="183"/>
+      <c r="AC1" s="183"/>
+      <c r="AD1" s="183"/>
+      <c r="AE1" s="183"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
@@ -4169,11 +4169,11 @@
       <c r="B4" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="182">
+      <c r="C4" s="185">
         <v>44459</v>
       </c>
-      <c r="D4" s="182"/>
-      <c r="E4" s="182"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
       <c r="F4" s="155"/>
       <c r="G4" s="105" t="s">
         <v>73</v>
@@ -4183,182 +4183,182 @@
       </c>
       <c r="I4" s="103"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="179" t="str">
+      <c r="K4" s="177" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="180"/>
-      <c r="M4" s="180"/>
-      <c r="N4" s="180"/>
-      <c r="O4" s="180"/>
-      <c r="P4" s="180"/>
-      <c r="Q4" s="181"/>
-      <c r="R4" s="179" t="str">
+      <c r="L4" s="178"/>
+      <c r="M4" s="178"/>
+      <c r="N4" s="178"/>
+      <c r="O4" s="178"/>
+      <c r="P4" s="178"/>
+      <c r="Q4" s="179"/>
+      <c r="R4" s="177" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="180"/>
-      <c r="T4" s="180"/>
-      <c r="U4" s="180"/>
-      <c r="V4" s="180"/>
-      <c r="W4" s="180"/>
-      <c r="X4" s="181"/>
-      <c r="Y4" s="179" t="str">
+      <c r="S4" s="178"/>
+      <c r="T4" s="178"/>
+      <c r="U4" s="178"/>
+      <c r="V4" s="178"/>
+      <c r="W4" s="178"/>
+      <c r="X4" s="179"/>
+      <c r="Y4" s="177" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="180"/>
-      <c r="AA4" s="180"/>
-      <c r="AB4" s="180"/>
-      <c r="AC4" s="180"/>
-      <c r="AD4" s="180"/>
-      <c r="AE4" s="181"/>
-      <c r="AF4" s="179" t="str">
+      <c r="Z4" s="178"/>
+      <c r="AA4" s="178"/>
+      <c r="AB4" s="178"/>
+      <c r="AC4" s="178"/>
+      <c r="AD4" s="178"/>
+      <c r="AE4" s="179"/>
+      <c r="AF4" s="177" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="180"/>
-      <c r="AH4" s="180"/>
-      <c r="AI4" s="180"/>
-      <c r="AJ4" s="180"/>
-      <c r="AK4" s="180"/>
-      <c r="AL4" s="181"/>
-      <c r="AM4" s="179" t="str">
+      <c r="AG4" s="178"/>
+      <c r="AH4" s="178"/>
+      <c r="AI4" s="178"/>
+      <c r="AJ4" s="178"/>
+      <c r="AK4" s="178"/>
+      <c r="AL4" s="179"/>
+      <c r="AM4" s="177" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="180"/>
-      <c r="AO4" s="180"/>
-      <c r="AP4" s="180"/>
-      <c r="AQ4" s="180"/>
-      <c r="AR4" s="180"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="179" t="str">
+      <c r="AN4" s="178"/>
+      <c r="AO4" s="178"/>
+      <c r="AP4" s="178"/>
+      <c r="AQ4" s="178"/>
+      <c r="AR4" s="178"/>
+      <c r="AS4" s="179"/>
+      <c r="AT4" s="177" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="180"/>
-      <c r="AV4" s="180"/>
-      <c r="AW4" s="180"/>
-      <c r="AX4" s="180"/>
-      <c r="AY4" s="180"/>
-      <c r="AZ4" s="181"/>
-      <c r="BA4" s="179" t="str">
+      <c r="AU4" s="178"/>
+      <c r="AV4" s="178"/>
+      <c r="AW4" s="178"/>
+      <c r="AX4" s="178"/>
+      <c r="AY4" s="178"/>
+      <c r="AZ4" s="179"/>
+      <c r="BA4" s="177" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="180"/>
-      <c r="BC4" s="180"/>
-      <c r="BD4" s="180"/>
-      <c r="BE4" s="180"/>
-      <c r="BF4" s="180"/>
-      <c r="BG4" s="181"/>
-      <c r="BH4" s="179" t="str">
+      <c r="BB4" s="178"/>
+      <c r="BC4" s="178"/>
+      <c r="BD4" s="178"/>
+      <c r="BE4" s="178"/>
+      <c r="BF4" s="178"/>
+      <c r="BG4" s="179"/>
+      <c r="BH4" s="177" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="180"/>
-      <c r="BJ4" s="180"/>
-      <c r="BK4" s="180"/>
-      <c r="BL4" s="180"/>
-      <c r="BM4" s="180"/>
-      <c r="BN4" s="181"/>
+      <c r="BI4" s="178"/>
+      <c r="BJ4" s="178"/>
+      <c r="BK4" s="178"/>
+      <c r="BL4" s="178"/>
+      <c r="BM4" s="178"/>
+      <c r="BN4" s="179"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="102"/>
       <c r="B5" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="178" t="s">
+      <c r="C5" s="184" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="178"/>
-      <c r="E5" s="178"/>
+      <c r="D5" s="184"/>
+      <c r="E5" s="184"/>
       <c r="F5" s="156"/>
       <c r="G5" s="104"/>
       <c r="H5" s="104"/>
       <c r="I5" s="104"/>
       <c r="J5" s="49"/>
-      <c r="K5" s="183">
+      <c r="K5" s="180">
         <f>K6</f>
         <v>44459</v>
       </c>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="184"/>
-      <c r="O5" s="184"/>
-      <c r="P5" s="184"/>
-      <c r="Q5" s="185"/>
-      <c r="R5" s="183">
+      <c r="L5" s="181"/>
+      <c r="M5" s="181"/>
+      <c r="N5" s="181"/>
+      <c r="O5" s="181"/>
+      <c r="P5" s="181"/>
+      <c r="Q5" s="182"/>
+      <c r="R5" s="180">
         <f>R6</f>
         <v>44466</v>
       </c>
-      <c r="S5" s="184"/>
-      <c r="T5" s="184"/>
-      <c r="U5" s="184"/>
-      <c r="V5" s="184"/>
-      <c r="W5" s="184"/>
-      <c r="X5" s="185"/>
-      <c r="Y5" s="183">
+      <c r="S5" s="181"/>
+      <c r="T5" s="181"/>
+      <c r="U5" s="181"/>
+      <c r="V5" s="181"/>
+      <c r="W5" s="181"/>
+      <c r="X5" s="182"/>
+      <c r="Y5" s="180">
         <f>Y6</f>
         <v>44473</v>
       </c>
-      <c r="Z5" s="184"/>
-      <c r="AA5" s="184"/>
-      <c r="AB5" s="184"/>
-      <c r="AC5" s="184"/>
-      <c r="AD5" s="184"/>
-      <c r="AE5" s="185"/>
-      <c r="AF5" s="183">
+      <c r="Z5" s="181"/>
+      <c r="AA5" s="181"/>
+      <c r="AB5" s="181"/>
+      <c r="AC5" s="181"/>
+      <c r="AD5" s="181"/>
+      <c r="AE5" s="182"/>
+      <c r="AF5" s="180">
         <f>AF6</f>
         <v>44480</v>
       </c>
-      <c r="AG5" s="184"/>
-      <c r="AH5" s="184"/>
-      <c r="AI5" s="184"/>
-      <c r="AJ5" s="184"/>
-      <c r="AK5" s="184"/>
-      <c r="AL5" s="185"/>
-      <c r="AM5" s="183">
+      <c r="AG5" s="181"/>
+      <c r="AH5" s="181"/>
+      <c r="AI5" s="181"/>
+      <c r="AJ5" s="181"/>
+      <c r="AK5" s="181"/>
+      <c r="AL5" s="182"/>
+      <c r="AM5" s="180">
         <f>AM6</f>
         <v>44487</v>
       </c>
-      <c r="AN5" s="184"/>
-      <c r="AO5" s="184"/>
-      <c r="AP5" s="184"/>
-      <c r="AQ5" s="184"/>
-      <c r="AR5" s="184"/>
-      <c r="AS5" s="185"/>
-      <c r="AT5" s="183">
+      <c r="AN5" s="181"/>
+      <c r="AO5" s="181"/>
+      <c r="AP5" s="181"/>
+      <c r="AQ5" s="181"/>
+      <c r="AR5" s="181"/>
+      <c r="AS5" s="182"/>
+      <c r="AT5" s="180">
         <f>AT6</f>
         <v>44494</v>
       </c>
-      <c r="AU5" s="184"/>
-      <c r="AV5" s="184"/>
-      <c r="AW5" s="184"/>
-      <c r="AX5" s="184"/>
-      <c r="AY5" s="184"/>
-      <c r="AZ5" s="185"/>
-      <c r="BA5" s="183">
+      <c r="AU5" s="181"/>
+      <c r="AV5" s="181"/>
+      <c r="AW5" s="181"/>
+      <c r="AX5" s="181"/>
+      <c r="AY5" s="181"/>
+      <c r="AZ5" s="182"/>
+      <c r="BA5" s="180">
         <f>BA6</f>
         <v>44501</v>
       </c>
-      <c r="BB5" s="184"/>
-      <c r="BC5" s="184"/>
-      <c r="BD5" s="184"/>
-      <c r="BE5" s="184"/>
-      <c r="BF5" s="184"/>
-      <c r="BG5" s="185"/>
-      <c r="BH5" s="183">
+      <c r="BB5" s="181"/>
+      <c r="BC5" s="181"/>
+      <c r="BD5" s="181"/>
+      <c r="BE5" s="181"/>
+      <c r="BF5" s="181"/>
+      <c r="BG5" s="182"/>
+      <c r="BH5" s="180">
         <f>BH6</f>
         <v>44508</v>
       </c>
-      <c r="BI5" s="184"/>
-      <c r="BJ5" s="184"/>
-      <c r="BK5" s="184"/>
-      <c r="BL5" s="184"/>
-      <c r="BM5" s="184"/>
-      <c r="BN5" s="185"/>
+      <c r="BI5" s="181"/>
+      <c r="BJ5" s="181"/>
+      <c r="BK5" s="181"/>
+      <c r="BL5" s="181"/>
+      <c r="BM5" s="181"/>
+      <c r="BN5" s="182"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
@@ -6161,7 +6161,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="62">
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="I23" s="63">
         <f t="shared" si="4"/>
@@ -6248,7 +6248,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="63">
         <f t="shared" si="4"/>
@@ -6333,7 +6333,9 @@
       <c r="G25" s="172">
         <v>4</v>
       </c>
-      <c r="H25" s="173"/>
+      <c r="H25" s="173">
+        <v>1</v>
+      </c>
       <c r="I25" s="174">
         <f t="shared" si="4"/>
         <v>2</v>
@@ -12635,6 +12637,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -12645,15 +12656,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H91:H100 H84:H85 H8:H79 H81">

</xml_diff>

<commit_message>
edited or completed work
</commit_message>
<xml_diff>
--- a/gantt-chart_L version 2.xlsx
+++ b/gantt-chart_L version 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HTCS5607\HTCS5607\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFB95DF-3E3A-4FFF-A5F7-830B003DD665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D763566-0871-42A4-9BF8-F3CEC69F4741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3171,24 +3171,6 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3196,9 +3178,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="45" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="45" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="45" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4046,8 +4046,8 @@
   <dimension ref="A1:BN92"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+      <pane ySplit="7" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N69" sqref="N69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4075,29 +4075,29 @@
       <c r="E1" s="152"/>
       <c r="F1" s="152"/>
       <c r="I1" s="121"/>
-      <c r="K1" s="183" t="s">
+      <c r="K1" s="177" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="183"/>
-      <c r="M1" s="183"/>
-      <c r="N1" s="183"/>
-      <c r="O1" s="183"/>
-      <c r="P1" s="183"/>
-      <c r="Q1" s="183"/>
-      <c r="R1" s="183"/>
-      <c r="S1" s="183"/>
-      <c r="T1" s="183"/>
-      <c r="U1" s="183"/>
-      <c r="V1" s="183"/>
-      <c r="W1" s="183"/>
-      <c r="X1" s="183"/>
-      <c r="Y1" s="183"/>
-      <c r="Z1" s="183"/>
-      <c r="AA1" s="183"/>
-      <c r="AB1" s="183"/>
-      <c r="AC1" s="183"/>
-      <c r="AD1" s="183"/>
-      <c r="AE1" s="183"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="177"/>
+      <c r="T1" s="177"/>
+      <c r="U1" s="177"/>
+      <c r="V1" s="177"/>
+      <c r="W1" s="177"/>
+      <c r="X1" s="177"/>
+      <c r="Y1" s="177"/>
+      <c r="Z1" s="177"/>
+      <c r="AA1" s="177"/>
+      <c r="AB1" s="177"/>
+      <c r="AC1" s="177"/>
+      <c r="AD1" s="177"/>
+      <c r="AE1" s="177"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="51" t="s">
@@ -4142,11 +4142,11 @@
       <c r="B4" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="185">
+      <c r="C4" s="182">
         <v>44459</v>
       </c>
-      <c r="D4" s="185"/>
-      <c r="E4" s="185"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="182"/>
       <c r="F4" s="155"/>
       <c r="G4" s="105" t="s">
         <v>73</v>
@@ -4156,182 +4156,182 @@
       </c>
       <c r="I4" s="103"/>
       <c r="J4" s="49"/>
-      <c r="K4" s="177" t="str">
+      <c r="K4" s="179" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="178"/>
-      <c r="M4" s="178"/>
-      <c r="N4" s="178"/>
-      <c r="O4" s="178"/>
-      <c r="P4" s="178"/>
-      <c r="Q4" s="179"/>
-      <c r="R4" s="177" t="str">
+      <c r="L4" s="180"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="180"/>
+      <c r="O4" s="180"/>
+      <c r="P4" s="180"/>
+      <c r="Q4" s="181"/>
+      <c r="R4" s="179" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="178"/>
-      <c r="T4" s="178"/>
-      <c r="U4" s="178"/>
-      <c r="V4" s="178"/>
-      <c r="W4" s="178"/>
-      <c r="X4" s="179"/>
-      <c r="Y4" s="177" t="str">
+      <c r="S4" s="180"/>
+      <c r="T4" s="180"/>
+      <c r="U4" s="180"/>
+      <c r="V4" s="180"/>
+      <c r="W4" s="180"/>
+      <c r="X4" s="181"/>
+      <c r="Y4" s="179" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="178"/>
-      <c r="AA4" s="178"/>
-      <c r="AB4" s="178"/>
-      <c r="AC4" s="178"/>
-      <c r="AD4" s="178"/>
-      <c r="AE4" s="179"/>
-      <c r="AF4" s="177" t="str">
+      <c r="Z4" s="180"/>
+      <c r="AA4" s="180"/>
+      <c r="AB4" s="180"/>
+      <c r="AC4" s="180"/>
+      <c r="AD4" s="180"/>
+      <c r="AE4" s="181"/>
+      <c r="AF4" s="179" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="178"/>
-      <c r="AH4" s="178"/>
-      <c r="AI4" s="178"/>
-      <c r="AJ4" s="178"/>
-      <c r="AK4" s="178"/>
-      <c r="AL4" s="179"/>
-      <c r="AM4" s="177" t="str">
+      <c r="AG4" s="180"/>
+      <c r="AH4" s="180"/>
+      <c r="AI4" s="180"/>
+      <c r="AJ4" s="180"/>
+      <c r="AK4" s="180"/>
+      <c r="AL4" s="181"/>
+      <c r="AM4" s="179" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="178"/>
-      <c r="AO4" s="178"/>
-      <c r="AP4" s="178"/>
-      <c r="AQ4" s="178"/>
-      <c r="AR4" s="178"/>
-      <c r="AS4" s="179"/>
-      <c r="AT4" s="177" t="str">
+      <c r="AN4" s="180"/>
+      <c r="AO4" s="180"/>
+      <c r="AP4" s="180"/>
+      <c r="AQ4" s="180"/>
+      <c r="AR4" s="180"/>
+      <c r="AS4" s="181"/>
+      <c r="AT4" s="179" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="178"/>
-      <c r="AV4" s="178"/>
-      <c r="AW4" s="178"/>
-      <c r="AX4" s="178"/>
-      <c r="AY4" s="178"/>
-      <c r="AZ4" s="179"/>
-      <c r="BA4" s="177" t="str">
+      <c r="AU4" s="180"/>
+      <c r="AV4" s="180"/>
+      <c r="AW4" s="180"/>
+      <c r="AX4" s="180"/>
+      <c r="AY4" s="180"/>
+      <c r="AZ4" s="181"/>
+      <c r="BA4" s="179" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="178"/>
-      <c r="BC4" s="178"/>
-      <c r="BD4" s="178"/>
-      <c r="BE4" s="178"/>
-      <c r="BF4" s="178"/>
-      <c r="BG4" s="179"/>
-      <c r="BH4" s="177" t="str">
+      <c r="BB4" s="180"/>
+      <c r="BC4" s="180"/>
+      <c r="BD4" s="180"/>
+      <c r="BE4" s="180"/>
+      <c r="BF4" s="180"/>
+      <c r="BG4" s="181"/>
+      <c r="BH4" s="179" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="178"/>
-      <c r="BJ4" s="178"/>
-      <c r="BK4" s="178"/>
-      <c r="BL4" s="178"/>
-      <c r="BM4" s="178"/>
-      <c r="BN4" s="179"/>
+      <c r="BI4" s="180"/>
+      <c r="BJ4" s="180"/>
+      <c r="BK4" s="180"/>
+      <c r="BL4" s="180"/>
+      <c r="BM4" s="180"/>
+      <c r="BN4" s="181"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="102"/>
       <c r="B5" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="184" t="s">
+      <c r="C5" s="178" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
       <c r="F5" s="156"/>
       <c r="G5" s="104"/>
       <c r="H5" s="104"/>
       <c r="I5" s="104"/>
       <c r="J5" s="49"/>
-      <c r="K5" s="180">
+      <c r="K5" s="183">
         <f>K6</f>
         <v>44459</v>
       </c>
-      <c r="L5" s="181"/>
-      <c r="M5" s="181"/>
-      <c r="N5" s="181"/>
-      <c r="O5" s="181"/>
-      <c r="P5" s="181"/>
-      <c r="Q5" s="182"/>
-      <c r="R5" s="180">
+      <c r="L5" s="184"/>
+      <c r="M5" s="184"/>
+      <c r="N5" s="184"/>
+      <c r="O5" s="184"/>
+      <c r="P5" s="184"/>
+      <c r="Q5" s="185"/>
+      <c r="R5" s="183">
         <f>R6</f>
         <v>44466</v>
       </c>
-      <c r="S5" s="181"/>
-      <c r="T5" s="181"/>
-      <c r="U5" s="181"/>
-      <c r="V5" s="181"/>
-      <c r="W5" s="181"/>
-      <c r="X5" s="182"/>
-      <c r="Y5" s="180">
+      <c r="S5" s="184"/>
+      <c r="T5" s="184"/>
+      <c r="U5" s="184"/>
+      <c r="V5" s="184"/>
+      <c r="W5" s="184"/>
+      <c r="X5" s="185"/>
+      <c r="Y5" s="183">
         <f>Y6</f>
         <v>44473</v>
       </c>
-      <c r="Z5" s="181"/>
-      <c r="AA5" s="181"/>
-      <c r="AB5" s="181"/>
-      <c r="AC5" s="181"/>
-      <c r="AD5" s="181"/>
-      <c r="AE5" s="182"/>
-      <c r="AF5" s="180">
+      <c r="Z5" s="184"/>
+      <c r="AA5" s="184"/>
+      <c r="AB5" s="184"/>
+      <c r="AC5" s="184"/>
+      <c r="AD5" s="184"/>
+      <c r="AE5" s="185"/>
+      <c r="AF5" s="183">
         <f>AF6</f>
         <v>44480</v>
       </c>
-      <c r="AG5" s="181"/>
-      <c r="AH5" s="181"/>
-      <c r="AI5" s="181"/>
-      <c r="AJ5" s="181"/>
-      <c r="AK5" s="181"/>
-      <c r="AL5" s="182"/>
-      <c r="AM5" s="180">
+      <c r="AG5" s="184"/>
+      <c r="AH5" s="184"/>
+      <c r="AI5" s="184"/>
+      <c r="AJ5" s="184"/>
+      <c r="AK5" s="184"/>
+      <c r="AL5" s="185"/>
+      <c r="AM5" s="183">
         <f>AM6</f>
         <v>44487</v>
       </c>
-      <c r="AN5" s="181"/>
-      <c r="AO5" s="181"/>
-      <c r="AP5" s="181"/>
-      <c r="AQ5" s="181"/>
-      <c r="AR5" s="181"/>
-      <c r="AS5" s="182"/>
-      <c r="AT5" s="180">
+      <c r="AN5" s="184"/>
+      <c r="AO5" s="184"/>
+      <c r="AP5" s="184"/>
+      <c r="AQ5" s="184"/>
+      <c r="AR5" s="184"/>
+      <c r="AS5" s="185"/>
+      <c r="AT5" s="183">
         <f>AT6</f>
         <v>44494</v>
       </c>
-      <c r="AU5" s="181"/>
-      <c r="AV5" s="181"/>
-      <c r="AW5" s="181"/>
-      <c r="AX5" s="181"/>
-      <c r="AY5" s="181"/>
-      <c r="AZ5" s="182"/>
-      <c r="BA5" s="180">
+      <c r="AU5" s="184"/>
+      <c r="AV5" s="184"/>
+      <c r="AW5" s="184"/>
+      <c r="AX5" s="184"/>
+      <c r="AY5" s="184"/>
+      <c r="AZ5" s="185"/>
+      <c r="BA5" s="183">
         <f>BA6</f>
         <v>44501</v>
       </c>
-      <c r="BB5" s="181"/>
-      <c r="BC5" s="181"/>
-      <c r="BD5" s="181"/>
-      <c r="BE5" s="181"/>
-      <c r="BF5" s="181"/>
-      <c r="BG5" s="182"/>
-      <c r="BH5" s="180">
+      <c r="BB5" s="184"/>
+      <c r="BC5" s="184"/>
+      <c r="BD5" s="184"/>
+      <c r="BE5" s="184"/>
+      <c r="BF5" s="184"/>
+      <c r="BG5" s="185"/>
+      <c r="BH5" s="183">
         <f>BH6</f>
         <v>44508</v>
       </c>
-      <c r="BI5" s="181"/>
-      <c r="BJ5" s="181"/>
-      <c r="BK5" s="181"/>
-      <c r="BL5" s="181"/>
-      <c r="BM5" s="181"/>
-      <c r="BN5" s="182"/>
+      <c r="BI5" s="184"/>
+      <c r="BJ5" s="184"/>
+      <c r="BK5" s="184"/>
+      <c r="BL5" s="184"/>
+      <c r="BM5" s="184"/>
+      <c r="BN5" s="185"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
@@ -8454,7 +8454,7 @@
         <v>4</v>
       </c>
       <c r="H50" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="63">
         <f t="shared" si="4"/>
@@ -8626,7 +8626,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="173">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I52" s="174">
         <f t="shared" si="4"/>
@@ -8711,7 +8711,9 @@
       <c r="G53" s="172">
         <v>1</v>
       </c>
-      <c r="H53" s="173"/>
+      <c r="H53" s="173">
+        <v>1</v>
+      </c>
       <c r="I53" s="174">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8795,7 +8797,9 @@
       <c r="G54" s="172">
         <v>1</v>
       </c>
-      <c r="H54" s="173"/>
+      <c r="H54" s="173">
+        <v>1</v>
+      </c>
       <c r="I54" s="174">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8879,7 +8883,9 @@
       <c r="G55" s="172">
         <v>1</v>
       </c>
-      <c r="H55" s="173"/>
+      <c r="H55" s="173">
+        <v>1</v>
+      </c>
       <c r="I55" s="174">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -8963,7 +8969,9 @@
       <c r="G56" s="172">
         <v>1</v>
       </c>
-      <c r="H56" s="173"/>
+      <c r="H56" s="173">
+        <v>1</v>
+      </c>
       <c r="I56" s="174">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -9047,7 +9055,9 @@
       <c r="G57" s="172">
         <v>1</v>
       </c>
-      <c r="H57" s="173"/>
+      <c r="H57" s="173">
+        <v>1</v>
+      </c>
       <c r="I57" s="174">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -9131,7 +9141,9 @@
       <c r="G58" s="172">
         <v>1</v>
       </c>
-      <c r="H58" s="173"/>
+      <c r="H58" s="173">
+        <v>1</v>
+      </c>
       <c r="I58" s="174">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -9215,7 +9227,9 @@
       <c r="G59" s="172">
         <v>2</v>
       </c>
-      <c r="H59" s="173"/>
+      <c r="H59" s="173">
+        <v>1</v>
+      </c>
       <c r="I59" s="174">
         <f t="shared" si="4"/>
         <v>2</v>
@@ -9369,11 +9383,11 @@
       </c>
       <c r="D61" s="116"/>
       <c r="E61" s="161">
-        <v>44491</v>
+        <v>44471</v>
       </c>
       <c r="F61" s="162">
         <f>IF(ISBLANK(E61)," - ",IF(G61=0,E61,E61+G61-1))</f>
-        <v>44503</v>
+        <v>44483</v>
       </c>
       <c r="G61" s="61">
         <v>13</v>
@@ -9455,19 +9469,21 @@
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="161">
-        <v>44491</v>
+        <v>44471</v>
       </c>
       <c r="F62" s="162">
-        <f t="shared" si="6"/>
-        <v>44491</v>
+        <f>IF(ISBLANK(E62)," - ",IF(G62=0,E62,E62+G62-1))</f>
+        <v>44471</v>
       </c>
       <c r="G62" s="61">
         <v>1</v>
       </c>
-      <c r="H62" s="62"/>
+      <c r="H62" s="62">
+        <v>1</v>
+      </c>
       <c r="I62" s="63">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" s="93"/>
       <c r="K62" s="99"/>
@@ -9539,17 +9555,17 @@
       </c>
       <c r="D63" s="116"/>
       <c r="E63" s="161">
-        <v>44491</v>
+        <v>44471</v>
       </c>
       <c r="F63" s="162">
         <f t="shared" ref="F63:F71" si="8">IF(ISBLANK(E63)," - ",IF(G63=0,E63,E63+G63-1))</f>
-        <v>44492</v>
+        <v>44473</v>
       </c>
       <c r="G63" s="61">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H63" s="62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" s="63">
         <f t="shared" si="4"/>
@@ -9625,11 +9641,11 @@
       </c>
       <c r="D64" s="116"/>
       <c r="E64" s="161">
-        <v>44492</v>
+        <v>44474</v>
       </c>
       <c r="F64" s="162">
         <f t="shared" si="8"/>
-        <v>44493</v>
+        <v>44475</v>
       </c>
       <c r="G64" s="61">
         <v>2</v>
@@ -9637,7 +9653,7 @@
       <c r="H64" s="62"/>
       <c r="I64" s="63">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J64" s="93"/>
       <c r="K64" s="99"/>
@@ -9709,11 +9725,11 @@
       </c>
       <c r="D65" s="116"/>
       <c r="E65" s="161">
-        <v>44493</v>
+        <v>44475</v>
       </c>
       <c r="F65" s="162">
         <f t="shared" si="8"/>
-        <v>44495</v>
+        <v>44477</v>
       </c>
       <c r="G65" s="61">
         <v>3</v>
@@ -9721,7 +9737,7 @@
       <c r="H65" s="62"/>
       <c r="I65" s="63">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J65" s="93"/>
       <c r="K65" s="99"/>
@@ -9877,19 +9893,21 @@
       </c>
       <c r="D67" s="116"/>
       <c r="E67" s="161">
-        <v>44497</v>
+        <v>44475</v>
       </c>
       <c r="F67" s="162">
         <f t="shared" si="8"/>
-        <v>44499</v>
+        <v>44477</v>
       </c>
       <c r="G67" s="61">
         <v>3</v>
       </c>
-      <c r="H67" s="62"/>
+      <c r="H67" s="62">
+        <v>1</v>
+      </c>
       <c r="I67" s="63">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J67" s="93"/>
       <c r="K67" s="99"/>
@@ -10128,20 +10146,18 @@
         <v>136</v>
       </c>
       <c r="D70" s="116"/>
-      <c r="E70" s="161">
-        <v>44502</v>
-      </c>
-      <c r="F70" s="162">
+      <c r="E70" s="161"/>
+      <c r="F70" s="162" t="str">
         <f t="shared" si="8"/>
-        <v>44503</v>
+        <v xml:space="preserve"> - </v>
       </c>
       <c r="G70" s="61">
         <v>2</v>
       </c>
       <c r="H70" s="62"/>
-      <c r="I70" s="63">
+      <c r="I70" s="63" t="str">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v xml:space="preserve"> - </v>
       </c>
       <c r="J70" s="93"/>
       <c r="K70" s="99"/>
@@ -11920,15 +11936,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -11939,6 +11946,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H82:H91 H75:H76 H72 H8:H70">
@@ -12044,7 +12060,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 A85:B85 A87:B87 B86 E26 E60 E72 E85:H87 G26:H26 G60:H60 G72:H72 G88:G91 H61 H63 H75 H76" unlockedFormula="1"/>
+    <ignoredError sqref="H9 A85:B85 A87:B87 B86 E26 E60 E72 E85:H87 G26:H26 G60:H60 G72:H72 G88:G91 H61 H75 H76" unlockedFormula="1"/>
     <ignoredError sqref="A72 A60 A26" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>

</xml_diff>